<commit_message>
Visut paikoilleen, ikkunan kokojen viimeistelyä, kommentteja?
</commit_message>
<xml_diff>
--- a/kenttien_nimeaminen.xlsx
+++ b/kenttien_nimeaminen.xlsx
@@ -104,13 +104,13 @@
     <t>Haukimureke, fenkolipeti</t>
   </si>
   <si>
-    <t>Mustajuuri-chevrepihvit,</t>
-  </si>
-  <si>
     <t>Peuran sisäfile, metsäsienirisotto</t>
   </si>
   <si>
     <t>Rosvopaisti lampaan potkasta, haudutetut juurekset</t>
+  </si>
+  <si>
+    <t>Mustajuuri-chevrepihvit, hiiliperunat</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B20"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,17 +608,17 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>